<commit_message>
Added the correct Latex template.
git-svn-id: file:///localdisk/subversion/inca/trunk/pubs@15048 7dba3f4a-8be6-0310-8b3b-b4fec25ea7f3
</commit_message>
<xml_diff>
--- a/papers/inca-analysis/Inca-Analysis-Results.xlsx
+++ b/papers/inca-analysis/Inca-Analysis-Results.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22810"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15000" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="myhadoop" localSheetId="1">Sheet2!$A$11</definedName>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="47">
   <si>
     <t>Network</t>
   </si>
@@ -134,6 +135,36 @@
   </si>
   <si>
     <t>batch-testjob</t>
+  </si>
+  <si>
+    <t>iu-xray (hpcc128)</t>
+  </si>
+  <si>
+    <t>% Passed Reports</t>
+  </si>
+  <si>
+    <t>Test name, resource</t>
+  </si>
+  <si>
+    <t>start date: 010111</t>
+  </si>
+  <si>
+    <t>iu-india (hpcc128)</t>
+  </si>
+  <si>
+    <t>iu-xray (hpcc256)</t>
+  </si>
+  <si>
+    <t>iu-xray (hpcc512)</t>
+  </si>
+  <si>
+    <t>iu-xray (hpcc672)</t>
+  </si>
+  <si>
+    <t>(05/12-09/12) failures</t>
+  </si>
+  <si>
+    <t>iu-india (hpcc256)</t>
   </si>
 </sst>
 </file>
@@ -1255,7 +1286,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView topLeftCell="C1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
@@ -1496,7 +1527,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="E65" sqref="E65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1642,4 +1673,92 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="28.83203125" customWidth="1"/>
+    <col min="2" max="2" width="20" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0.93</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0.93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0.79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0.91</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0.93</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" s="1">
+        <v>0.99</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Latest results including reliability.
git-svn-id: file:///localdisk/subversion/inca/trunk/pubs@15050 7dba3f4a-8be6-0310-8b3b-b4fec25ea7f3
</commit_message>
<xml_diff>
--- a/papers/inca-analysis/Inca-Analysis-Results.xlsx
+++ b/papers/inca-analysis/Inca-Analysis-Results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22810"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15000" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="40" yWindow="0" windowWidth="48000" windowHeight="26420" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,16 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="myhadoop" localSheetId="1">Sheet2!$A$11</definedName>
+    <definedName name="hpcc128" localSheetId="1">Sheet2!$A$51</definedName>
+    <definedName name="hpcc16" localSheetId="1">Sheet2!$A$48</definedName>
+    <definedName name="hpcc256" localSheetId="1">Sheet2!$A$52</definedName>
+    <definedName name="hpcc32" localSheetId="1">Sheet2!$A$49</definedName>
+    <definedName name="hpcc512" localSheetId="1">Sheet2!$A$53</definedName>
+    <definedName name="hpcc64" localSheetId="1">Sheet2!$A$50</definedName>
+    <definedName name="hpcc672" localSheetId="1">Sheet2!$A$54</definedName>
+    <definedName name="hpcc8" localSheetId="1">Sheet2!$A$47</definedName>
+    <definedName name="myhadoop" localSheetId="1">Sheet2!#REF!</definedName>
+    <definedName name="vampirtrace" localSheetId="1">Sheet2!$A$57</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -24,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="79">
   <si>
     <t>Network</t>
   </si>
@@ -119,9 +128,6 @@
     <t>ucsd-sierra</t>
   </si>
   <si>
-    <t>The following nodes have leftover hadoop jobs</t>
-  </si>
-  <si>
     <t>stdout file does not exist or is empty</t>
   </si>
   <si>
@@ -165,13 +171,112 @@
   </si>
   <si>
     <t>iu-india (hpcc256)</t>
+  </si>
+  <si>
+    <t>ufl-foxtrot</t>
+  </si>
+  <si>
+    <t>OpenStack</t>
+  </si>
+  <si>
+    <t>cloud client not in running status after 1800 seconds</t>
+  </si>
+  <si>
+    <t>Command 'euca-run-instances  -k userkey -n 1 emi-FF7D1540 -t c1.medium' failed with exit code 1</t>
+  </si>
+  <si>
+    <t>Page Error</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>iu-bravo</t>
+  </si>
+  <si>
+    <t>iu-delta</t>
+  </si>
+  <si>
+    <t>batch-testjob_to_bravo</t>
+  </si>
+  <si>
+    <t>Job failed - data file /N/u/inca/Hadoop-Outputs/part-r-00000 is zero length</t>
+  </si>
+  <si>
+    <t>The following nodes have leftover hadoop jobs,</t>
+  </si>
+  <si>
+    <t>Job failed - data file /N/u/inca/Hadoop-Outputs/part-r-00000 does not exist</t>
+  </si>
+  <si>
+    <t>BATCH: Unable to submit reporter perl /N/u/inca/incaReporterManager/sub17331.pl:  qsub: Unauthorized Request  MSG=user ACL rejected the submitting user: user inca@i136, queue delta</t>
+  </si>
+  <si>
+    <t>BATCH: Unable to retrieve reporter output: No such file or directory</t>
+  </si>
+  <si>
+    <t>hpcc8</t>
+  </si>
+  <si>
+    <t>hpcc16</t>
+  </si>
+  <si>
+    <t>hpcc32</t>
+  </si>
+  <si>
+    <t>hpcc64</t>
+  </si>
+  <si>
+    <t>hpcc128</t>
+  </si>
+  <si>
+    <t>hpcc256</t>
+  </si>
+  <si>
+    <t>hpcc512</t>
+  </si>
+  <si>
+    <t>hpcc672</t>
+  </si>
+  <si>
+    <t>Unable to download http://inca.futuregrid.org/repository/share/fg-alamo-hpccinf.txt.8.v1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No output file hpccoutf.txt found: </t>
+  </si>
+  <si>
+    <t>No output in hpccoutf.txt</t>
+  </si>
+  <si>
+    <t>No output file hpccoutf.txt</t>
+  </si>
+  <si>
+    <t>vampirtrace</t>
+  </si>
+  <si>
+    <t>env MPICH_FAST_MEMCPY=1 MPICH_PTL_MATCH_OFF=1 aprun -N 8 -ss -cc cpu  -n 4 failed:  aprun: -N cannot exceed -n</t>
+  </si>
+  <si>
+    <t>aprun: Exiting due to errors. Application aborted</t>
+  </si>
+  <si>
+    <t>ring-man not found</t>
+  </si>
+  <si>
+    <t>mpirun -np 4 failed: No such file or directory</t>
+  </si>
+  <si>
+    <t>' /opt/xcat/sbin/dumpxCATdb --version' failed: No such file or directory</t>
+  </si>
+  <si>
+    <t>xcat</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -200,6 +305,75 @@
       <color theme="1"/>
       <name val="Courier"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Courier"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Courier"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Courier"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF3366FF"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF3366FF"/>
+      <name val="Courier"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF008000"/>
+      <name val="Courier"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF008000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF800000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF800000"/>
+      <name val="Courier"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -218,7 +392,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="13">
+  <cellStyleXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -232,8 +406,40 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -242,20 +448,83 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="13">
+  <cellStyles count="45">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -345,11 +614,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2082851176"/>
-        <c:axId val="2082854184"/>
+        <c:axId val="2103751800"/>
+        <c:axId val="2103748776"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2082851176"/>
+        <c:axId val="2103751800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -358,7 +627,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2082854184"/>
+        <c:crossAx val="2103748776"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -366,7 +635,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2082854184"/>
+        <c:axId val="2103748776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -377,14 +646,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2082851176"/>
+        <c:crossAx val="2103751800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -499,11 +767,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2082913992"/>
-        <c:axId val="2082916936"/>
+        <c:axId val="2103692440"/>
+        <c:axId val="2103689480"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2082913992"/>
+        <c:axId val="2103692440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -512,7 +780,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2082916936"/>
+        <c:crossAx val="2103689480"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -520,7 +788,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2082916936"/>
+        <c:axId val="2103689480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -531,14 +799,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2082913992"/>
+        <c:crossAx val="2103692440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -641,11 +908,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2082940712"/>
-        <c:axId val="2082943720"/>
+        <c:axId val="2103665720"/>
+        <c:axId val="2103662696"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2082940712"/>
+        <c:axId val="2103665720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -654,7 +921,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2082943720"/>
+        <c:crossAx val="2103662696"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -662,7 +929,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2082943720"/>
+        <c:axId val="2103662696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -673,14 +940,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2082940712"/>
+        <c:crossAx val="2103665720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -783,11 +1049,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2082967416"/>
-        <c:axId val="2082970424"/>
+        <c:axId val="2103638984"/>
+        <c:axId val="2103635960"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2082967416"/>
+        <c:axId val="2103638984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -796,7 +1062,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2082970424"/>
+        <c:crossAx val="2103635960"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -804,7 +1070,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2082970424"/>
+        <c:axId val="2103635960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -815,14 +1081,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2082967416"/>
+        <c:crossAx val="2103638984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1524,18 +1789,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:N61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E65" sqref="E65"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="19" customWidth="1"/>
+    <col min="1" max="1" width="38.33203125" customWidth="1"/>
+    <col min="2" max="2" width="16.1640625" customWidth="1"/>
+    <col min="8" max="8" width="10.83203125" customWidth="1"/>
+    <col min="10" max="10" width="58.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:6">
       <c r="B1" t="s">
         <v>22</v>
       </c>
@@ -1546,122 +1814,541 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
-      <c r="A2" t="s">
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B5" s="1">
         <v>0.98</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C5" s="1">
         <v>0.92</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D5" s="1">
         <v>0.97</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
-      <c r="A3" t="s">
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B6" s="1">
         <v>0.92</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C6" s="1">
         <v>0.79</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D6" s="1">
         <v>0.65</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
-      <c r="A4" t="s">
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B7" s="1">
         <v>1</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C7" s="1">
         <v>0.83</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D7" s="1">
         <v>0.76</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
-      <c r="B9" t="s">
+    <row r="14" spans="1:6">
+      <c r="A14" s="7">
+        <v>40544</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D15" s="2"/>
+      <c r="E15" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F15" s="2"/>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="1">
+        <v>0.96</v>
+      </c>
+      <c r="E16" s="1">
+        <v>0.93</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="A17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" s="1">
+        <v>0.77</v>
+      </c>
+      <c r="E17" s="1">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="K17" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
+      <c r="A18" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
+      <c r="A20" s="7">
+        <v>40544</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
+      <c r="A21" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D21" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E21" s="2" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" t="s">
-        <v>36</v>
-      </c>
-      <c r="B10" s="1">
+      <c r="F21" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
+      <c r="A22" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22" s="1">
+        <v>0.98</v>
+      </c>
+      <c r="D22" s="1">
+        <v>0.96</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="F22" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="J22" s="6"/>
+      <c r="L22" s="5"/>
+    </row>
+    <row r="23" spans="1:12">
+      <c r="A23" t="s">
+        <v>26</v>
+      </c>
+      <c r="C23" s="1">
+        <v>0.93</v>
+      </c>
+      <c r="D23" s="1">
+        <v>0.89</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="F23" s="1">
+        <v>0.57999999999999996</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12">
+      <c r="A24" t="s">
+        <v>27</v>
+      </c>
+      <c r="C24" s="1">
         <v>1</v>
       </c>
-      <c r="C10" s="1">
+      <c r="D24" s="1">
+        <v>0.97</v>
+      </c>
+      <c r="E24" s="1">
+        <v>0.98</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12">
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+    </row>
+    <row r="26" spans="1:12">
+      <c r="A26" s="7">
+        <v>40544</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12">
+      <c r="A27" t="s">
+        <v>47</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F27" s="2"/>
+    </row>
+    <row r="28" spans="1:12">
+      <c r="A28" t="s">
+        <v>25</v>
+      </c>
+      <c r="B28" s="1">
+        <v>0.97</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12">
+      <c r="A29" t="s">
+        <v>26</v>
+      </c>
+      <c r="B29" s="1">
+        <v>0.71</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12">
+      <c r="A30" t="s">
+        <v>27</v>
+      </c>
+      <c r="B30" s="1">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14">
+      <c r="A34" s="7">
+        <v>40544</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14">
+      <c r="B35" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14">
+      <c r="A36" t="s">
+        <v>35</v>
+      </c>
+      <c r="D36" s="1">
+        <v>0.88</v>
+      </c>
+      <c r="E36" s="1">
+        <v>0.97</v>
+      </c>
+      <c r="F36" s="1">
+        <v>0.77</v>
+      </c>
+      <c r="G36" s="1">
+        <v>1</v>
+      </c>
+      <c r="H36" s="1">
         <v>0.99</v>
       </c>
-      <c r="D10" s="1">
-        <v>1</v>
-      </c>
-      <c r="E10" s="1">
-        <v>1</v>
-      </c>
-      <c r="G10" s="3" t="s">
+      <c r="J36" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14">
+      <c r="A37" t="s">
+        <v>54</v>
+      </c>
+      <c r="B37" s="1">
+        <v>0.99</v>
+      </c>
+      <c r="J37" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14">
+      <c r="A38" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" t="s">
+      <c r="C38" s="1">
+        <v>0.95</v>
+      </c>
+      <c r="J38" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14">
+      <c r="A39" t="s">
+        <v>33</v>
+      </c>
+      <c r="C39" s="1">
+        <v>0.95</v>
+      </c>
+      <c r="J39" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14">
+      <c r="A40" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="1">
-        <v>0.53</v>
-      </c>
-      <c r="C11" s="1">
-        <v>0.82</v>
-      </c>
-      <c r="D11" s="1">
+      <c r="D40" s="1">
+        <v>0.54</v>
+      </c>
+      <c r="F40" s="1">
+        <v>0.59</v>
+      </c>
+      <c r="G40" s="1">
         <v>0.89</v>
       </c>
-      <c r="E11" s="1">
-        <v>0.39</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" t="s">
-        <v>33</v>
-      </c>
-      <c r="B12" s="1">
+      <c r="H40" s="1">
+        <v>0.47</v>
+      </c>
+      <c r="J40" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14">
+      <c r="J41" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14">
+      <c r="J42" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14">
+      <c r="K43" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14">
+      <c r="A45" s="7">
+        <v>40544</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14">
+      <c r="A46" s="2"/>
+      <c r="B46" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G46" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H46" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14">
+      <c r="A47" t="s">
+        <v>60</v>
+      </c>
+      <c r="D47" s="1">
+        <v>0.99</v>
+      </c>
+      <c r="E47" s="1">
+        <v>0.97</v>
+      </c>
+      <c r="F47" s="8">
+        <v>0</v>
+      </c>
+      <c r="G47" s="10">
+        <v>0</v>
+      </c>
+      <c r="H47" s="1">
+        <v>0.72</v>
+      </c>
+      <c r="J47" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="N47" s="11" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14">
+      <c r="A48" t="s">
+        <v>61</v>
+      </c>
+      <c r="D48" s="1">
+        <v>0.99</v>
+      </c>
+      <c r="E48" s="1">
+        <v>0.96</v>
+      </c>
+      <c r="J48" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13">
+      <c r="A49" t="s">
+        <v>62</v>
+      </c>
+      <c r="E49" s="1">
         <v>0.95</v>
       </c>
-      <c r="G12" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" t="s">
-        <v>34</v>
-      </c>
-      <c r="B13" s="1">
-        <v>0.95</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>35</v>
+      <c r="J49" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13">
+      <c r="A50" t="s">
+        <v>63</v>
+      </c>
+      <c r="D50" s="1">
+        <v>0.97</v>
+      </c>
+      <c r="E50" s="1">
+        <v>0.96</v>
+      </c>
+      <c r="J50" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13">
+      <c r="A51" t="s">
+        <v>64</v>
+      </c>
+      <c r="D51" s="1">
+        <v>0.93</v>
+      </c>
+      <c r="E51" s="1">
+        <v>0.93</v>
+      </c>
+      <c r="J51" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13">
+      <c r="A52" t="s">
+        <v>65</v>
+      </c>
+      <c r="D52" s="1">
+        <v>0.79</v>
+      </c>
+      <c r="E52" s="1">
+        <v>0.91</v>
+      </c>
+      <c r="J52" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13">
+      <c r="A53" t="s">
+        <v>66</v>
+      </c>
+      <c r="E53" s="1">
+        <v>0.93</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13">
+      <c r="A54" t="s">
+        <v>67</v>
+      </c>
+      <c r="E54" s="1">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13">
+      <c r="A57" s="12">
+        <v>40544</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="J57" s="9" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13">
+      <c r="A58" t="s">
+        <v>72</v>
+      </c>
+      <c r="B58" s="8">
+        <v>0</v>
+      </c>
+      <c r="C58" s="13">
+        <v>0</v>
+      </c>
+      <c r="D58" s="16">
+        <v>0</v>
+      </c>
+      <c r="E58" s="17">
+        <v>0</v>
+      </c>
+      <c r="J58" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="K58" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="M58" s="15" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13">
+      <c r="J59" s="18" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13">
+      <c r="A61" t="s">
+        <v>78</v>
+      </c>
+      <c r="E61" s="1">
+        <v>0.97</v>
+      </c>
+      <c r="J61" s="3" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -1679,7 +2366,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -1691,23 +2378,23 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B3" s="1">
         <v>0.93</v>
@@ -1715,7 +2402,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B4" s="1">
         <v>0.93</v>
@@ -1723,7 +2410,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B5" s="1">
         <v>0.79</v>
@@ -1731,7 +2418,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B6" s="1">
         <v>0.91</v>
@@ -1739,7 +2426,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B7" s="1">
         <v>0.93</v>
@@ -1747,7 +2434,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B8" s="1">
         <v>0.99</v>

</xml_diff>

<commit_message>
Added more figures on cloud reliability and performance.
git-svn-id: file:///localdisk/subversion/inca/trunk/pubs@15053 7dba3f4a-8be6-0310-8b3b-b4fec25ea7f3
</commit_message>
<xml_diff>
--- a/papers/inca-analysis/Inca-Analysis-Results.xlsx
+++ b/papers/inca-analysis/Inca-Analysis-Results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22810"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="40" yWindow="0" windowWidth="48000" windowHeight="26420" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="2480" yWindow="420" windowWidth="48000" windowHeight="26480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <definedName name="hpcc672" localSheetId="1">Sheet2!$A$54</definedName>
     <definedName name="hpcc8" localSheetId="1">Sheet2!$A$47</definedName>
     <definedName name="myhadoop" localSheetId="1">Sheet2!#REF!</definedName>
-    <definedName name="vampirtrace" localSheetId="1">Sheet2!$A$57</definedName>
+    <definedName name="vampirtrace" localSheetId="1">Sheet2!#REF!</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="70">
   <si>
     <t>Network</t>
   </si>
@@ -239,44 +239,17 @@
     <t>hpcc672</t>
   </si>
   <si>
-    <t>Unable to download http://inca.futuregrid.org/repository/share/fg-alamo-hpccinf.txt.8.v1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No output file hpccoutf.txt found: </t>
-  </si>
-  <si>
     <t>No output in hpccoutf.txt</t>
   </si>
   <si>
     <t>No output file hpccoutf.txt</t>
-  </si>
-  <si>
-    <t>vampirtrace</t>
-  </si>
-  <si>
-    <t>env MPICH_FAST_MEMCPY=1 MPICH_PTL_MATCH_OFF=1 aprun -N 8 -ss -cc cpu  -n 4 failed:  aprun: -N cannot exceed -n</t>
-  </si>
-  <si>
-    <t>aprun: Exiting due to errors. Application aborted</t>
-  </si>
-  <si>
-    <t>ring-man not found</t>
-  </si>
-  <si>
-    <t>mpirun -np 4 failed: No such file or directory</t>
-  </si>
-  <si>
-    <t>' /opt/xcat/sbin/dumpxCATdb --version' failed: No such file or directory</t>
-  </si>
-  <si>
-    <t>xcat</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -339,39 +312,6 @@
     <font>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
-      <name val="Courier"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF3366FF"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF3366FF"/>
-      <name val="Courier"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF008000"/>
-      <name val="Courier"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF008000"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF800000"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF800000"/>
       <name val="Courier"/>
     </font>
   </fonts>
@@ -439,7 +379,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -462,21 +402,6 @@
     </xf>
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="9" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -556,6 +481,11 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+          </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
@@ -651,10 +581,6 @@
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -691,6 +617,11 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+          </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
@@ -804,10 +735,6 @@
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -844,6 +771,11 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+          </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
@@ -945,10 +877,6 @@
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -985,6 +913,11 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+          </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
@@ -1088,6 +1021,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1106,16 +1040,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>795868</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:rowOff>173567</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>622300</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
+      <xdr:colOff>588434</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>55034</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1551,8 +1485,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B59"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1789,10 +1723,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N61"/>
+  <dimension ref="A1:N54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1959,8 +1893,8 @@
       <c r="D23" s="1">
         <v>0.89</v>
       </c>
-      <c r="E23" s="6" t="s">
-        <v>50</v>
+      <c r="E23" s="1">
+        <v>0.91</v>
       </c>
       <c r="F23" s="1">
         <v>0.57999999999999996</v>
@@ -2003,9 +1937,7 @@
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
-      <c r="E27" s="4" t="s">
-        <v>30</v>
-      </c>
+      <c r="E27" s="4"/>
       <c r="F27" s="2"/>
     </row>
     <row r="28" spans="1:12">
@@ -2170,12 +2102,8 @@
       <c r="E46" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F46" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="G46" s="2" t="s">
-        <v>13</v>
-      </c>
+      <c r="F46" s="2"/>
+      <c r="G46" s="2"/>
       <c r="H46" s="2" t="s">
         <v>30</v>
       </c>
@@ -2190,21 +2118,13 @@
       <c r="E47" s="1">
         <v>0.97</v>
       </c>
-      <c r="F47" s="8">
-        <v>0</v>
-      </c>
-      <c r="G47" s="10">
-        <v>0</v>
-      </c>
+      <c r="F47" s="8"/>
+      <c r="G47" s="10"/>
       <c r="H47" s="1">
         <v>0.72</v>
       </c>
-      <c r="J47" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="N47" s="11" t="s">
-        <v>69</v>
-      </c>
+      <c r="J47" s="9"/>
+      <c r="N47" s="11"/>
     </row>
     <row r="48" spans="1:14">
       <c r="A48" t="s">
@@ -2217,10 +2137,10 @@
         <v>0.96</v>
       </c>
       <c r="J48" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="49" spans="1:13">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10">
       <c r="A49" t="s">
         <v>62</v>
       </c>
@@ -2228,10 +2148,10 @@
         <v>0.95</v>
       </c>
       <c r="J49" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="50" spans="1:13">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10">
       <c r="A50" t="s">
         <v>63</v>
       </c>
@@ -2242,10 +2162,10 @@
         <v>0.96</v>
       </c>
       <c r="J50" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="51" spans="1:13">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10">
       <c r="A51" t="s">
         <v>64</v>
       </c>
@@ -2256,10 +2176,10 @@
         <v>0.93</v>
       </c>
       <c r="J51" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="52" spans="1:13">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10">
       <c r="A52" t="s">
         <v>65</v>
       </c>
@@ -2270,10 +2190,10 @@
         <v>0.91</v>
       </c>
       <c r="J52" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="53" spans="1:13">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10">
       <c r="A53" t="s">
         <v>66</v>
       </c>
@@ -2281,74 +2201,12 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="54" spans="1:13">
+    <row r="54" spans="1:10">
       <c r="A54" t="s">
         <v>67</v>
       </c>
       <c r="E54" s="1">
         <v>0.99</v>
-      </c>
-    </row>
-    <row r="57" spans="1:13">
-      <c r="A57" s="12">
-        <v>40544</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D57" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E57" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="J57" s="9" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="58" spans="1:13">
-      <c r="A58" t="s">
-        <v>72</v>
-      </c>
-      <c r="B58" s="8">
-        <v>0</v>
-      </c>
-      <c r="C58" s="13">
-        <v>0</v>
-      </c>
-      <c r="D58" s="16">
-        <v>0</v>
-      </c>
-      <c r="E58" s="17">
-        <v>0</v>
-      </c>
-      <c r="J58" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="K58" s="14" t="s">
-        <v>75</v>
-      </c>
-      <c r="M58" s="15" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="59" spans="1:13">
-      <c r="J59" s="18" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="61" spans="1:13">
-      <c r="A61" t="s">
-        <v>78</v>
-      </c>
-      <c r="E61" s="1">
-        <v>0.97</v>
-      </c>
-      <c r="J61" s="3" t="s">
-        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>